<commit_message>
Xception 수정(base model trainable)
</commit_message>
<xml_diff>
--- a/model_summary_5epoch.xlsx
+++ b/model_summary_5epoch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonWorkspace\220307-0715_AI전문가과정\AI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA14D295-B9C7-47E2-8822-CBC44B79436A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294842D2-4181-4066-9191-0C2FAEB26E6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="372" yWindow="0" windowWidth="11412" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -461,8 +461,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" x14ac:dyDescent="0.65"/>
@@ -670,16 +670,16 @@
         <v>5</v>
       </c>
       <c r="F7" s="1">
-        <v>0.90200000000000002</v>
+        <v>0.91090000000000004</v>
       </c>
       <c r="G7" s="1">
-        <v>0.90776145458221402</v>
+        <v>0.92132353782653797</v>
       </c>
       <c r="H7" s="3">
-        <v>0.3634</v>
+        <v>0.371</v>
       </c>
       <c r="I7" s="3">
-        <v>0.33320459723472501</v>
+        <v>0.29586303234100297</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
unseen class 추가 14개 class_EffNetV2M_Test acc 84.08%
</commit_message>
<xml_diff>
--- a/model_summary_5epoch.xlsx
+++ b/model_summary_5epoch.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonWorkspace\220307-0715_AI전문가과정\AI_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\작업방\AI교육\팀프로젝트\GitHub\AI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC818BD4-755E-428C-A272-80C74AF6367C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="0" windowWidth="11412" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="370" yWindow="0" windowWidth="11410" windowHeight="8880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>개발일시</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -95,12 +94,24 @@
   </si>
   <si>
     <t>CoAtNet0</t>
+  </si>
+  <si>
+    <t>박영서</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>비고</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>unseen('맛집' 검색) class acc 51%로 낮음</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="0.0000_ "/>
   </numFmts>
@@ -468,28 +479,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="7.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.84765625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.3984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.8984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.8984375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="12.09765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.3984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.4140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.9140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.9140625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="12.08203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.4140625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.84765625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.84765625" style="4"/>
+    <col min="9" max="9" width="7.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.33203125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -517,8 +529,11 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.65">
+      <c r="J1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="5">
         <v>220608</v>
       </c>
@@ -547,7 +562,7 @@
         <v>7.6215036213397896E-2</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="5">
         <v>220609</v>
       </c>
@@ -576,7 +591,7 @@
         <v>0.37890000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="5">
         <v>220609</v>
       </c>
@@ -605,7 +620,7 @@
         <v>0.71160000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>220609</v>
       </c>
@@ -634,7 +649,7 @@
         <v>0.51290000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="5">
         <v>220614</v>
       </c>
@@ -663,7 +678,7 @@
         <v>0.20861004292964899</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="5">
         <v>220614</v>
       </c>
@@ -692,7 +707,7 @@
         <v>0.29586303234100297</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="5">
         <v>220614</v>
       </c>
@@ -721,7 +736,7 @@
         <v>0.33320459723472501</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="5">
         <v>220614</v>
       </c>
@@ -750,7 +765,7 @@
         <v>0.55012446641921997</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="5">
         <v>220617</v>
       </c>
@@ -777,6 +792,38 @@
       </c>
       <c r="I10" s="3">
         <v>0.96923035383224398</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A11" s="5">
+        <v>220620</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>14</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.87139999999999995</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.84079999999999999</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.56289999999999996</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.59319999999999995</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
model summary 수정 (soft max사용)
</commit_message>
<xml_diff>
--- a/model_summary_5epoch.xlsx
+++ b/model_summary_5epoch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonWorkspace\220307-0715_AI전문가과정\AI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC818BD4-755E-428C-A272-80C74AF6367C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55AE8D0-C785-4AC9-9A0B-5C858A0F5D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="372" yWindow="0" windowWidth="11412" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="15552" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" x14ac:dyDescent="0.65"/>
@@ -665,7 +665,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A7" s="5">
-        <v>220614</v>
+        <v>220622</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>10</v>
@@ -680,21 +680,21 @@
         <v>5</v>
       </c>
       <c r="F7" s="1">
-        <v>0.91090000000000004</v>
+        <v>0.89100000000000001</v>
       </c>
       <c r="G7" s="1">
-        <v>0.92132353782653797</v>
+        <v>0.90882354974746704</v>
       </c>
       <c r="H7" s="3">
-        <v>0.371</v>
+        <v>0.36499999999999999</v>
       </c>
       <c r="I7" s="3">
-        <v>0.29586303234100297</v>
+        <v>0.32725152373313898</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A8" s="5">
-        <v>220614</v>
+        <v>220622</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -709,21 +709,21 @@
         <v>5</v>
       </c>
       <c r="F8" s="1">
-        <v>0.88009999999999999</v>
+        <v>0.83440000000000003</v>
       </c>
       <c r="G8" s="1">
-        <v>0.90776145458221402</v>
+        <v>0.86307191848754805</v>
       </c>
       <c r="H8" s="3">
-        <v>0.61150000000000004</v>
+        <v>0.55679000000000001</v>
       </c>
       <c r="I8" s="3">
-        <v>0.33320459723472501</v>
+        <v>0.48514580726623502</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.65">
       <c r="A9" s="5">
-        <v>220614</v>
+        <v>220622</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>15</v>
@@ -738,16 +738,16 @@
         <v>5</v>
       </c>
       <c r="F9" s="1">
-        <v>0.86780000000000002</v>
+        <v>0.86370000000000002</v>
       </c>
       <c r="G9" s="1">
-        <v>0.87549018859863204</v>
+        <v>0.87181371450424106</v>
       </c>
       <c r="H9" s="3">
-        <v>0.50539999999999996</v>
+        <v>1.7292000000000001</v>
       </c>
       <c r="I9" s="3">
-        <v>0.55012446641921997</v>
+        <v>0.811184883117675</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.65">

</xml_diff>

<commit_message>
17class 모델, ensemble 코드 추가
</commit_message>
<xml_diff>
--- a/model_summary_5epoch.xlsx
+++ b/model_summary_5epoch.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonWorkspace\220307-0715_AI전문가과정\AI_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55AE8D0-C785-4AC9-9A0B-5C858A0F5D34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F37A65-A6A2-4A9D-8033-9BF3DD73D17D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="15552" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$14</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
   <si>
     <t>개발일시</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -469,10 +472,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84765625" defaultRowHeight="15" x14ac:dyDescent="0.65"/>
@@ -779,8 +783,137 @@
         <v>0.96923035383224398</v>
       </c>
     </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.65">
+      <c r="A11" s="5">
+        <v>220623</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="2">
+        <v>17</v>
+      </c>
+      <c r="E11" s="2">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.89510000000000001</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.88880000000000003</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0.43430000000000002</v>
+      </c>
+      <c r="I11" s="3">
+        <v>0.53180000000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.65">
+      <c r="A12" s="5">
+        <v>220623</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" s="2">
+        <v>17</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.87419999999999998</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.874048471450805</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.76770000000000005</v>
+      </c>
+      <c r="I12" s="3">
+        <v>0.75166046619415205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.65">
+      <c r="A13" s="5">
+        <v>220623</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2">
+        <v>17</v>
+      </c>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.78</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.76257210969924905</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0.96660000000000001</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1.3760806322097701</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.65">
+      <c r="A14" s="5">
+        <v>220623</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2">
+        <v>17</v>
+      </c>
+      <c r="E14" s="2">
+        <v>5</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.83709999999999996</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.824221432209014</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0.77080000000000004</v>
+      </c>
+      <c r="I14" s="3">
+        <v>0.89661860466003396</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:I14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="F2:G1048576">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>